<commit_message>
Editorial fixes for workbook and checklist
</commit_message>
<xml_diff>
--- a/manage/opsmanagementworkbook.xlsx
+++ b/manage/opsmanagementworkbook.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brblanch\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68858034-F751-42E5-B08D-263D7B28E773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74E632F-67CD-40F1-A4C7-CEA443D3D390}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{879A4F07-C4C9-4C02-9DE6-A381B214C244}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{879A4F07-C4C9-4C02-9DE6-A381B214C244}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="4" r:id="rId1"/>
@@ -24,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
   <si>
     <t>Microsoft Cloud Adoption Framework for Azure</t>
   </si>
@@ -48,30 +44,15 @@
     <t>Standard Commitment</t>
   </si>
   <si>
-    <t>Comitment Level</t>
-  </si>
-  <si>
     <t>Alternative time frames may be more applicable.</t>
   </si>
   <si>
-    <t>Time/Value impact*</t>
-  </si>
-  <si>
-    <t>* Time/Value Impact based on revenue losses per hour of downtime</t>
-  </si>
-  <si>
-    <t>** Composite SLA of the deployed solution, not a single asset</t>
-  </si>
-  <si>
     <t>Composite SLA**</t>
   </si>
   <si>
     <t>Est. Outage***</t>
   </si>
   <si>
-    <t xml:space="preserve">*** Estimated outage based on hours per year. </t>
-  </si>
-  <si>
     <t>Monthly Cost</t>
   </si>
   <si>
@@ -174,9 +155,6 @@
     <t>Annual ROI****</t>
   </si>
   <si>
-    <t>**** Annual ROI is a compartive figure to understand if the cost of the level of commitment produces a return based on forecasted outages</t>
-  </si>
-  <si>
     <t>Standard Impact</t>
   </si>
   <si>
@@ -184,6 +162,30 @@
   </si>
   <si>
     <t>Commitment level impact*</t>
+  </si>
+  <si>
+    <t>Time/Value Impact*</t>
+  </si>
+  <si>
+    <t>Commitment Level</t>
+  </si>
+  <si>
+    <t>Commitment Level Impact*</t>
+  </si>
+  <si>
+    <t>Comparison Basis</t>
+  </si>
+  <si>
+    <t>* Time/Value Impact based on revenue losses per hour of downtime.</t>
+  </si>
+  <si>
+    <t>** Composite SLA of the deployed solution, not a single asset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** Estimated Outage based on hours per year. </t>
+  </si>
+  <si>
+    <t>**** Annual ROI is a comparative figure to understand if the cost of the level of commitment produces a return based on forecasted outages.</t>
   </si>
 </sst>
 </file>
@@ -192,9 +194,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -265,31 +267,178 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.0000%"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -328,7 +477,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -353,7 +502,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="171" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -380,112 +529,7 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="171" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
     </dxf>
     <dxf>
       <font>
@@ -506,25 +550,17 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.0000%"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,28 +576,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F6A2410B-A25B-492D-899B-74CF55BB3C1B}" name="Table13" displayName="Table13" ref="A5:K29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F6A2410B-A25B-492D-899B-74CF55BB3C1B}" name="Table13" displayName="Table13" ref="A5:K29" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A5:K29" xr:uid="{17AF3D0B-5E62-47BC-A927-4D08E9D9FB6C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{EBFA83CC-6557-4087-940A-A5D130D98B29}" name="Workload"/>
     <tableColumn id="2" xr3:uid="{75F5E97D-7130-45AB-B5AE-BE2BB6E39AC8}" name="Criticality"/>
-    <tableColumn id="3" xr3:uid="{7E42CCF8-035D-42A0-B75C-34F266B608DE}" name="Time/Value impact*"/>
-    <tableColumn id="4" xr3:uid="{7A73F4F2-5A78-483B-88BD-0EB3317B55A7}" name="Comitment Level" dataDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{AD0B2E4C-3FF2-49DF-B6F0-E60F09FE461E}" name="Composite SLA**" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{7E42CCF8-035D-42A0-B75C-34F266B608DE}" name="Time/Value Impact*"/>
+    <tableColumn id="4" xr3:uid="{7A73F4F2-5A78-483B-88BD-0EB3317B55A7}" name="Commitment Level" dataDxfId="17" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{AD0B2E4C-3FF2-49DF-B6F0-E60F09FE461E}" name="Composite SLA**" dataDxfId="16" dataCellStyle="Percent"/>
     <tableColumn id="5" xr3:uid="{2AEACCB4-AFA1-460C-BD82-02EC56451832}" name="Monthly Cost" dataDxfId="15" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{7EE80C8F-45A7-4045-8B14-1B97FAC9964F}" name="Est. Outage***" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{7EE80C8F-45A7-4045-8B14-1B97FAC9964F}" name="Est. Outage***" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F1EFBB97-67B8-47AE-AD31-A5BE5ACB7989}" name="Standard Impact" dataDxfId="10" dataCellStyle="Currency">
-      <calculatedColumnFormula>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{F1EFBB97-67B8-47AE-AD31-A5BE5ACB7989}" name="Standard Impact" dataDxfId="13" dataCellStyle="Currency">
+      <calculatedColumnFormula>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{118F6C5B-0D31-4366-9F05-66958B0905F5}" name="Commitment level impact*" dataDxfId="11" dataCellStyle="Currency">
-      <calculatedColumnFormula>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{118F6C5B-0D31-4366-9F05-66958B0905F5}" name="Commitment level impact*" dataDxfId="12" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{03DA4F84-2B11-456C-9870-C06B208CE05A}" name="Comparison basis" dataDxfId="14" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{03DA4F84-2B11-456C-9870-C06B208CE05A}" name="Comparison basis" dataDxfId="11" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(Table13[[#This Row],[Standard Impact]]=Table13[[#This Row],[Commitment level impact*]], Table13[[#This Row],[Standard Impact]], Table13[[#This Row],[Standard Impact]]-Table13[[#This Row],[Commitment level impact*]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2360698A-BE65-4FEA-9583-1E0B13479D87}" name="Annual ROI****" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="9" xr3:uid="{2360698A-BE65-4FEA-9583-1E0B13479D87}" name="Annual ROI****" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table13[[#This Row],[Comparison basis]]-(Table13[[#This Row],[Monthly Cost]]*12))/(Table13[[#This Row],[Monthly Cost]]*12)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -570,29 +606,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E129EBD0-5652-4D18-9DF1-763F608EEA1C}" name="Table134" displayName="Table134" ref="A5:K29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E129EBD0-5652-4D18-9DF1-763F608EEA1C}" name="Table134" displayName="Table134" ref="A5:K29" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Currency">
   <autoFilter ref="A5:K29" xr:uid="{17AF3D0B-5E62-47BC-A927-4D08E9D9FB6C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B6C4564B-7435-4A5D-AB64-59237DD14D12}" name="Workload"/>
     <tableColumn id="2" xr3:uid="{2936D3EF-3A76-4BE6-973F-687A21176158}" name="Criticality"/>
-    <tableColumn id="3" xr3:uid="{0AE0259E-639E-4E6A-B56F-16320868F6B7}" name="Time/Value impact*"/>
-    <tableColumn id="4" xr3:uid="{CD2C4AC5-8238-4C5E-9505-AC4B23484755}" name="Comitment Level" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{539FFF17-A0A5-4230-9069-8525814044E3}" name="Composite SLA**" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{3169ED64-8277-4EDF-9282-F54A87D2B520}" name="Monthly Cost" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{87EE16D9-ED5E-4217-9A19-6FDC28DE1608}" name="Est. Outage***" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{0AE0259E-639E-4E6A-B56F-16320868F6B7}" name="Time/Value Impact*"/>
+    <tableColumn id="4" xr3:uid="{CD2C4AC5-8238-4C5E-9505-AC4B23484755}" name="Commitment Level" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{539FFF17-A0A5-4230-9069-8525814044E3}" name="Composite SLA**" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{3169ED64-8277-4EDF-9282-F54A87D2B520}" name="Monthly Cost" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{87EE16D9-ED5E-4217-9A19-6FDC28DE1608}" name="Est. Outage***" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0C8B433B-6863-4519-9EBA-F497726BFF22}" name="Standard Impact" dataDxfId="4" dataCellStyle="Currency">
-      <calculatedColumnFormula>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{0C8B433B-6863-4519-9EBA-F497726BFF22}" name="Standard Impact" dataDxfId="3" dataCellStyle="Currency">
+      <calculatedColumnFormula>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAD60C6E-BD6A-43A3-AF88-01C4D828D325}" name="Commitment level impact*" dataDxfId="3" dataCellStyle="Currency">
-      <calculatedColumnFormula>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{EAD60C6E-BD6A-43A3-AF88-01C4D828D325}" name="Commitment Level Impact*" dataDxfId="2" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{FE258315-0E1D-47DC-B404-6F178618F724}" name="Comparison basis" dataDxfId="2" dataCellStyle="Currency">
-      <calculatedColumnFormula>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</calculatedColumnFormula>
+    <tableColumn id="12" xr3:uid="{FE258315-0E1D-47DC-B404-6F178618F724}" name="Comparison Basis" dataDxfId="1" dataCellStyle="Currency">
+      <calculatedColumnFormula>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BC29E757-6FED-4FC4-B598-2CE8A4C97F2A}" name="Annual ROI****" dataDxfId="1" dataCellStyle="Percent">
-      <calculatedColumnFormula>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{BC29E757-6FED-4FC4-B598-2CE8A4C97F2A}" name="Annual ROI****" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -898,104 +934,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30E9CF5-6E86-4CBF-9D81-60573761EF20}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.08984375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" customWidth="1"/>
-    <col min="15" max="15" width="42.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="61.77734375" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="15" width="42.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="M4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="I5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="K5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>1000000</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3">
         <v>0.99999899999999997</v>
@@ -1007,12 +1040,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000002518996E-3</v>
       </c>
-      <c r="H6" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H6" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760000.0000000093</v>
       </c>
       <c r="I6" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>8760.0000002518991</v>
       </c>
       <c r="J6" s="6">
@@ -1024,24 +1057,24 @@
         <v>6.2926999999997983</v>
       </c>
       <c r="M6" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="N6">
         <v>8760</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4">
         <v>1000000</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3">
         <v>0.99999000000000005</v>
@@ -1053,12 +1086,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.759999999960133E-2</v>
       </c>
-      <c r="H7" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H7" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760000.0000000093</v>
       </c>
       <c r="I7" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>87599.999999601336</v>
       </c>
       <c r="J7" s="6">
@@ -1070,21 +1103,21 @@
         <v>23.090000000001133</v>
       </c>
       <c r="M7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
         <v>200000</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3">
         <v>0.99990000000000001</v>
@@ -1096,12 +1129,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>0.87599999999990352</v>
       </c>
-      <c r="H8" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H8" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>1752000.0000000016</v>
       </c>
       <c r="I8" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>175199.9999999807</v>
       </c>
       <c r="J8" s="6">
@@ -1113,18 +1146,18 @@
         <v>130.40000000000174</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4">
         <v>10000</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3">
         <v>0.99950000000000006</v>
@@ -1136,12 +1169,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>4.3799999999995176</v>
       </c>
-      <c r="H9" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H9" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="I9" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43799.999999995176</v>
       </c>
       <c r="J9" s="6">
@@ -1153,15 +1186,15 @@
         <v>2.6500000000004094</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4">
         <v>10000</v>
@@ -1179,12 +1212,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H10" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H10" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="I10" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="J10" s="6">
@@ -1196,12 +1229,12 @@
         <v>72.000000000000071</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4">
         <v>10000</v>
@@ -1219,12 +1252,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H11" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H11" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="I11" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="J11" s="6">
@@ -1236,12 +1269,12 @@
         <v>72.000000000000071</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4">
         <v>10000</v>
@@ -1259,12 +1292,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H12" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H12" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="I12" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>87600.000000000087</v>
       </c>
       <c r="J12" s="6">
@@ -1276,12 +1309,12 @@
         <v>72.000000000000071</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4">
         <v>5000</v>
@@ -1299,12 +1332,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H13" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H13" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="I13" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="J13" s="6">
@@ -1316,12 +1349,12 @@
         <v>35.500000000000036</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4">
         <v>5000</v>
@@ -1339,12 +1372,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H14" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H14" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="I14" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="J14" s="6">
@@ -1356,12 +1389,12 @@
         <v>35.500000000000036</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15" s="4">
         <v>5000</v>
@@ -1379,12 +1412,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H15" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H15" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="I15" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="J15" s="6">
@@ -1396,12 +1429,12 @@
         <v>35.500000000000036</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4">
         <v>5000</v>
@@ -1419,12 +1452,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H16" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H16" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="I16" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="J16" s="6">
@@ -1436,12 +1469,12 @@
         <v>35.500000000000036</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4">
         <v>5000</v>
@@ -1459,12 +1492,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H17" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H17" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="I17" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>43800.000000000044</v>
       </c>
       <c r="J17" s="6">
@@ -1476,12 +1509,12 @@
         <v>35.500000000000036</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4">
         <v>1000</v>
@@ -1499,12 +1532,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H18" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H18" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="I18" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="J18" s="6">
@@ -1516,12 +1549,12 @@
         <v>6.3000000000000078</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4">
         <v>1000</v>
@@ -1539,12 +1572,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H19" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H19" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="I19" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="J19" s="6">
@@ -1556,12 +1589,12 @@
         <v>6.3000000000000078</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4">
         <v>1000</v>
@@ -1579,12 +1612,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H20" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H20" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="I20" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="J20" s="6">
@@ -1596,12 +1629,12 @@
         <v>6.3000000000000078</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C21" s="4">
         <v>1000</v>
@@ -1619,12 +1652,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H21" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H21" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="I21" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>8760.0000000000091</v>
       </c>
       <c r="J21" s="6">
@@ -1636,12 +1669,12 @@
         <v>-0.96350000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4">
         <v>0</v>
@@ -1659,12 +1692,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H22" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H22" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I22" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J22" s="6">
@@ -1676,12 +1709,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4">
         <v>0</v>
@@ -1699,12 +1732,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H23" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H23" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I23" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J23" s="6">
@@ -1716,12 +1749,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4">
         <v>0</v>
@@ -1739,12 +1772,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H24" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H24" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I24" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J24" s="6">
@@ -1756,12 +1789,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
       </c>
       <c r="C25" s="4">
         <v>0</v>
@@ -1779,12 +1812,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H25" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H25" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I25" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J25" s="6">
@@ -1796,12 +1829,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C26" s="4">
         <v>0</v>
@@ -1819,12 +1852,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H26" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H26" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I26" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J26" s="6">
@@ -1836,12 +1869,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
@@ -1859,12 +1892,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H27" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H27" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I27" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J27" s="6">
@@ -1876,12 +1909,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
@@ -1899,12 +1932,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H28" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H28" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I28" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J28" s="6">
@@ -1916,12 +1949,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
@@ -1939,12 +1972,12 @@
         <f>(1-Table13[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H29" s="10">
-        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value impact*]]</f>
+      <c r="H29" s="8">
+        <f>(1-0.999)*$N$6*Table13[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I29" s="6">
-        <f>Table13[[#This Row],[Time/Value impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
+        <f>Table13[[#This Row],[Time/Value Impact*]]*Table13[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J29" s="6">
@@ -1963,6 +1996,9 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="K6:K29">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1974,9 +2010,6 @@
           <x14:id>{F9FD3E54-F1B0-4506-B24F-0F873D3C7C97}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThanOrEqual">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2010,93 +2043,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C4FB48-5DB8-4EDA-A7F6-20ECCB47C7C7}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.08984375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" customWidth="1"/>
-    <col min="15" max="15" width="42.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" customWidth="1"/>
+    <col min="13" max="13" width="61.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="M4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C6" s="4">
         <v>0</v>
       </c>
@@ -2111,30 +2139,30 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H6" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H6" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I6" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J6" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K6" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M6" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="N6">
         <v>8760</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C7" s="4">
         <v>0</v>
       </c>
@@ -2149,27 +2177,27 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H7" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H7" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I7" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J7" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K7" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C8" s="4">
         <v>0</v>
       </c>
@@ -2184,24 +2212,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H8" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H8" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I8" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J8" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K8" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" s="4">
         <v>0</v>
       </c>
@@ -2216,27 +2244,27 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H9" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H9" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I9" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J9" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K9" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>0</v>
       </c>
@@ -2251,24 +2279,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H10" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H10" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I10" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J10" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K10" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" s="4">
         <v>0</v>
       </c>
@@ -2283,24 +2311,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H11" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H11" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I11" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J11" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K11" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C12" s="4">
         <v>0</v>
       </c>
@@ -2315,24 +2343,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H12" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H12" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I12" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J12" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K12" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" s="4">
         <v>0</v>
       </c>
@@ -2347,24 +2375,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H13" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H13" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I13" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J13" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K13" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="4">
         <v>0</v>
       </c>
@@ -2379,24 +2407,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H14" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H14" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I14" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J14" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K14" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" s="4">
         <v>0</v>
       </c>
@@ -2411,24 +2439,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H15" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H15" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I15" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J15" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K15" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C16" s="4">
         <v>0</v>
       </c>
@@ -2443,24 +2471,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H16" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H16" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I16" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J16" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K16" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" s="4">
         <v>0</v>
       </c>
@@ -2475,24 +2503,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H17" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H17" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I17" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J17" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K17" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="4">
         <v>0</v>
       </c>
@@ -2507,24 +2535,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H18" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H18" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I18" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J18" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K18" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" s="4">
         <v>0</v>
       </c>
@@ -2539,24 +2567,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H19" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H19" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I19" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J19" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K19" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="4">
         <v>0</v>
       </c>
@@ -2571,24 +2599,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H20" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H20" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I20" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J20" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K20" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="4">
         <v>0</v>
       </c>
@@ -2603,24 +2631,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H21" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H21" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I21" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J21" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K21" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" s="4">
         <v>0</v>
       </c>
@@ -2635,24 +2663,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H22" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H22" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I22" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J22" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K22" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C23" s="4">
         <v>0</v>
       </c>
@@ -2667,24 +2695,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H23" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H23" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I23" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J23" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K23" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C24" s="4">
         <v>0</v>
       </c>
@@ -2699,24 +2727,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H24" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H24" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I24" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J24" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K24" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C25" s="4">
         <v>0</v>
       </c>
@@ -2731,24 +2759,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H25" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H25" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I25" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J25" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K25" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26" s="4">
         <v>0</v>
       </c>
@@ -2763,24 +2791,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H26" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H26" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I26" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J26" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K26" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C27" s="4">
         <v>0</v>
       </c>
@@ -2795,24 +2823,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H27" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H27" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I27" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J27" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K27" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C28" s="4">
         <v>0</v>
       </c>
@@ -2827,24 +2855,24 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H28" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H28" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I28" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J28" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K28" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C29" s="4">
         <v>0</v>
       </c>
@@ -2859,20 +2887,20 @@
         <f>(1-Table134[[#This Row],[Composite SLA**]])*$N$6</f>
         <v>8.7600000000000087</v>
       </c>
-      <c r="H29" s="10">
-        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value impact*]]</f>
+      <c r="H29" s="8">
+        <f>(1-0.999)*$N$6*Table134[[#This Row],[Time/Value Impact*]]</f>
         <v>0</v>
       </c>
       <c r="I29" s="6">
-        <f>Table134[[#This Row],[Time/Value impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
+        <f>Table134[[#This Row],[Time/Value Impact*]]*Table134[[#This Row],[Est. Outage***]]</f>
         <v>0</v>
       </c>
       <c r="J29" s="6">
-        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment level impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment level impact*]])</f>
+        <f>IF(Table134[[#This Row],[Standard Impact]]=Table134[[#This Row],[Commitment Level Impact*]], Table134[[#This Row],[Standard Impact]], Table134[[#This Row],[Standard Impact]]-Table134[[#This Row],[Commitment Level Impact*]])</f>
         <v>0</v>
       </c>
       <c r="K29" s="2" t="e">
-        <f>(Table134[[#This Row],[Comparison basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
+        <f>(Table134[[#This Row],[Comparison Basis]]-(Table134[[#This Row],[Monthly Cost]]*12))/(Table134[[#This Row],[Monthly Cost]]*12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2882,7 +2910,7 @@
     <mergeCell ref="D4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="K6:K29">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="dataBar" priority="2">

</xml_diff>